<commit_message>
updated the coordination sheet
</commit_message>
<xml_diff>
--- a/documentations/2023 coordination sheet.xlsx
+++ b/documentations/2023 coordination sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2023-prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BF8B41-707B-4E11-85DE-0A4F1B5EFF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70119DC-E32A-4DAD-91B1-572AF70C548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
   <si>
     <t>Relay Function Chart</t>
   </si>
@@ -68,15 +68,6 @@
     </r>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Br</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -145,16 +136,10 @@
     <t xml:space="preserve">Motor and Relay Coordination Chart including Functions </t>
   </si>
   <si>
-    <t>Talon SRX</t>
-  </si>
-  <si>
     <t>CAN</t>
   </si>
   <si>
     <t>Joystick</t>
-  </si>
-  <si>
-    <t>y-axis</t>
   </si>
   <si>
     <t>Joystick 0</t>
@@ -392,15 +377,6 @@
     <t>Joystick0 - Arcade Drive</t>
   </si>
   <si>
-    <t>x-axis</t>
-  </si>
-  <si>
-    <t>x negated so &gt;0 CCW</t>
-  </si>
-  <si>
-    <t>Y negated so &gt;0 forward</t>
-  </si>
-  <si>
     <t>Turbo mode</t>
   </si>
   <si>
@@ -410,19 +386,7 @@
     <t>so forward is  positive y and CCW rotation is positive X</t>
   </si>
   <si>
-    <t>Or</t>
-  </si>
-  <si>
-    <t>ID-6</t>
-  </si>
-  <si>
     <t>Joystick 1 - Operator</t>
-  </si>
-  <si>
-    <t>Gn</t>
-  </si>
-  <si>
-    <t>PDP 2</t>
   </si>
   <si>
     <t>PDP 1</t>
@@ -649,39 +613,6 @@
     <t>Inverted (yes/no)/sensor phase (true/false)</t>
   </si>
   <si>
-    <t>Bag motor</t>
-  </si>
-  <si>
-    <t>mini CIM</t>
-  </si>
-  <si>
-    <t>ID-7</t>
-  </si>
-  <si>
-    <t>ID-8</t>
-  </si>
-  <si>
-    <t>ID-11</t>
-  </si>
-  <si>
-    <t>Bu</t>
-  </si>
-  <si>
-    <t>PDP 3</t>
-  </si>
-  <si>
-    <t>PDP 4</t>
-  </si>
-  <si>
-    <t>PDP 5</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Br-R</t>
-  </si>
-  <si>
     <t>Vision Processing</t>
   </si>
   <si>
@@ -706,9 +637,6 @@
     <t>Roborio Port 0</t>
   </si>
   <si>
-    <t>Br-Bk</t>
-  </si>
-  <si>
     <t>Drive straight</t>
   </si>
   <si>
@@ -796,18 +724,6 @@
     <t>Ball Storage 2</t>
   </si>
   <si>
-    <t>Gy</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>PL 0</t>
-  </si>
-  <si>
-    <t>ID-5</t>
-  </si>
-  <si>
     <t>Ball Storage 1</t>
   </si>
   <si>
@@ -851,48 +767,6 @@
   </si>
   <si>
     <t>PDP 19</t>
-  </si>
-  <si>
-    <t>Ball intake motor left</t>
-  </si>
-  <si>
-    <t>Ball intake motor right slave</t>
-  </si>
-  <si>
-    <t>Pl Gy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Ball Beltcro</t>
-  </si>
-  <si>
-    <t>Electromagnets</t>
-  </si>
-  <si>
-    <t>magnet</t>
-  </si>
-  <si>
-    <t>relay</t>
-  </si>
-  <si>
-    <t>Spike</t>
-  </si>
-  <si>
-    <t>Relay 0</t>
-  </si>
-  <si>
-    <t>PDP 6</t>
-  </si>
-  <si>
-    <t>ID-10</t>
-  </si>
-  <si>
-    <t>PDP 16</t>
-  </si>
-  <si>
-    <t>PDP 17</t>
   </si>
   <si>
     <r>
@@ -911,21 +785,6 @@
     </r>
   </si>
   <si>
-    <t>Magnet climb lock grabby arms</t>
-  </si>
-  <si>
-    <t>Servo</t>
-  </si>
-  <si>
-    <t>PWM</t>
-  </si>
-  <si>
-    <t>PWM-0</t>
-  </si>
-  <si>
-    <t>Or-Y</t>
-  </si>
-  <si>
     <t>Climb Camera</t>
   </si>
   <si>
@@ -944,68 +803,56 @@
     <t>SPI</t>
   </si>
   <si>
-    <t>Climb hook left</t>
-  </si>
-  <si>
-    <t>Climb hook right</t>
-  </si>
-  <si>
-    <t>vertical climb motor left</t>
-  </si>
-  <si>
-    <t>vertical climb motor right</t>
-  </si>
-  <si>
-    <t>pigeon (vinnie)</t>
-  </si>
-  <si>
-    <t>ID-12</t>
-  </si>
-  <si>
-    <t>PDP 10</t>
-  </si>
-  <si>
-    <t>Ball Shooter Bottom</t>
-  </si>
-  <si>
-    <t>Ball Shooter Top</t>
-  </si>
-  <si>
-    <t>Ball Shooter Tiny wheels</t>
-  </si>
-  <si>
-    <t>(p)775</t>
-  </si>
-  <si>
-    <t>Some encoder thingy</t>
-  </si>
-  <si>
-    <t>ID - 6</t>
-  </si>
-  <si>
-    <t>ID-13</t>
-  </si>
-  <si>
-    <t>ID-14</t>
-  </si>
-  <si>
     <t>PDP 18</t>
   </si>
   <si>
-    <t>PDP 15</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>PDP 13</t>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Using Logitech Controller</t>
+  </si>
+  <si>
+    <t>Drive north/south</t>
+  </si>
+  <si>
+    <t>Drive east/west</t>
+  </si>
+  <si>
+    <t>left y-axis</t>
+  </si>
+  <si>
+    <t>right x-axis</t>
+  </si>
+  <si>
+    <t>DEFAULT manual drive command</t>
+  </si>
+  <si>
+    <t>Both Joystick drive mode</t>
+  </si>
+  <si>
+    <t>left joystick</t>
+  </si>
+  <si>
+    <t>Turret</t>
+  </si>
+  <si>
+    <t>Direction Pad</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1144,22 +991,6 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1181,7 +1012,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1476,56 +1307,6 @@
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1673,7 +1454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1759,84 +1540,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1845,178 +1595,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2048,13 +1762,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>417635</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>3395</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2091,13 +1805,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2113,8 +1827,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12161519" y="10166986"/>
-          <a:ext cx="1781176" cy="1655445"/>
+          <a:off x="12152049" y="8238386"/>
+          <a:ext cx="1778957" cy="1674088"/>
           <a:chOff x="10410824" y="9220200"/>
           <a:chExt cx="1771651" cy="1933575"/>
         </a:xfrm>
@@ -3094,6 +2808,56 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>64156</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>143059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>74490</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>92772</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB678DE-9D7A-82A4-C5D8-AB801D303CE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4464091" y="12593156"/>
+          <a:ext cx="5504109" cy="2161970"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3606,17 +3370,17 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="69" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="55" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
@@ -3631,12 +3395,12 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="88"/>
+        <v>20</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="72"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -3651,1135 +3415,885 @@
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="56" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="H4" s="9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M4" s="27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="24">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="I5" s="102">
+        <v>158</v>
+      </c>
+      <c r="I5" s="84">
         <v>40</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="24">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>21</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>77</v>
+        <v>160</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="102">
+        <v>70</v>
+      </c>
+      <c r="I6" s="84">
         <v>40</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I7" s="84">
+        <v>40</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I7" s="102">
-        <v>40</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="K7" s="12" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="84">
+        <v>40</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="90"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1">
+      <c r="D10" s="83"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="D11" s="83"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
+      <c r="A13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="24">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="24">
+        <v>10</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="22"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="24">
+        <v>3</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="24">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="22"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="D18" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="24">
+        <v>5</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="24">
+        <v>6</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="22"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="32">
+        <v>7</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="22"/>
+    </row>
+    <row r="21" spans="1:13" hidden="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="22"/>
+    </row>
+    <row r="22" spans="1:13" hidden="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="22"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="24">
+        <v>11</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="22"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="24">
+        <v>8</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="22"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1">
+      <c r="A25" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="23">
         <v>9</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="102">
-        <v>40</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="10">
-        <v>30</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" s="10">
-        <v>30</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="111" customFormat="1">
-      <c r="A11" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="B11" s="106" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="107" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="108" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="109" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="109" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="109" t="s">
-        <v>211</v>
-      </c>
-      <c r="I11" s="109">
-        <v>30</v>
-      </c>
-      <c r="J11" s="109" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="106" t="s">
-        <v>169</v>
-      </c>
-      <c r="L11" s="109"/>
-      <c r="M11" s="110"/>
-    </row>
-    <row r="12" spans="1:13" s="111" customFormat="1">
-      <c r="A12" s="105" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="106" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="107" t="s">
-        <v>186</v>
-      </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="109" t="s">
-        <v>187</v>
-      </c>
-      <c r="F12" s="109" t="s">
-        <v>188</v>
-      </c>
-      <c r="G12" s="109" t="s">
-        <v>160</v>
-      </c>
-      <c r="H12" s="109" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="109">
-        <v>20</v>
-      </c>
-      <c r="J12" s="109"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="109"/>
-      <c r="M12" s="110"/>
-    </row>
-    <row r="13" spans="1:13" ht="24">
-      <c r="A13" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="I13" s="102">
-        <v>40</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="24">
-      <c r="A14" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="B14" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="32">
-        <v>40</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="33"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="B15" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="33"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="B16" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="33"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="B17" s="101" t="s">
-        <v>215</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="33"/>
-    </row>
-    <row r="18" spans="1:13" ht="24">
-      <c r="A18" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="I18" s="103">
-        <v>40</v>
-      </c>
-      <c r="J18" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="33"/>
-    </row>
-    <row r="19" spans="1:13" s="111" customFormat="1">
-      <c r="A19" s="112" t="s">
-        <v>194</v>
-      </c>
-      <c r="B19" s="113" t="s">
-        <v>195</v>
-      </c>
-      <c r="C19" s="107" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" s="108"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="109" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="H19" s="113" t="s">
-        <v>196</v>
-      </c>
-      <c r="I19" s="114"/>
-      <c r="J19" s="113" t="s">
-        <v>120</v>
-      </c>
-      <c r="K19" s="106"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="115"/>
-    </row>
-    <row r="20" spans="1:13" ht="24.6" thickBot="1">
-      <c r="A20" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" s="104">
-        <v>40</v>
-      </c>
-      <c r="J20" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="29"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="89"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A22" s="65"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
-      <c r="A24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="9" t="s">
+      <c r="F25" s="15"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="23"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" hidden="1" thickTop="1">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" hidden="1" thickBot="1">
+      <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="28"/>
+    </row>
+    <row r="28" spans="1:13" ht="84.6" hidden="1" thickTop="1">
+      <c r="A28" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="29"/>
+    </row>
+    <row r="29" spans="1:13" hidden="1">
+      <c r="A29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="24">
-        <v>2</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C26" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="24">
-        <v>10</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="24">
-        <v>3</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="24">
-        <v>4</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="22"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="83" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="24">
-        <v>5</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="K29" s="10"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" hidden="1">
       <c r="A30" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="E30" s="24">
-        <v>6</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="22"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="K30" s="10"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" hidden="1">
       <c r="A31" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" s="36">
-        <v>7</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="22"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:13" hidden="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="10"/>
+      <c r="A32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="22"/>
-    </row>
-    <row r="33" spans="1:13" hidden="1">
-      <c r="A33" s="3"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12" hidden="1">
+      <c r="A33" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="73"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="10"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="22"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="K33" s="10"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:12" hidden="1">
       <c r="A34" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E34" s="24">
-        <v>11</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="10"/>
+        <v>80</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="22"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C35" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="24">
-        <v>8</v>
-      </c>
-      <c r="F35" s="14"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" hidden="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="48"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" thickBot="1">
-      <c r="A36" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C36" s="74" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="E36" s="23">
+      <c r="K35" s="10"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" hidden="1" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.6" hidden="1" thickTop="1" thickBot="1">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="25"/>
+    </row>
+    <row r="38" spans="1:12" ht="101.4" hidden="1" thickTop="1">
+      <c r="A38" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="23"/>
-    </row>
-    <row r="37" spans="1:13" ht="15" hidden="1" thickTop="1">
-      <c r="D37" s="1"/>
-      <c r="L37" s="65"/>
-    </row>
-    <row r="38" spans="1:13" ht="15" hidden="1" thickBot="1">
-      <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="18"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="28"/>
-    </row>
-    <row r="39" spans="1:13" ht="84.6" hidden="1" thickTop="1">
-      <c r="A39" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="9" t="s">
+      <c r="D38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="K38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" s="30"/>
-    </row>
-    <row r="40" spans="1:13" hidden="1">
-      <c r="A40" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="L38" s="29"/>
+    </row>
+    <row r="39" spans="1:12" hidden="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10">
+        <v>12</v>
+      </c>
+      <c r="K39" s="10"/>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" hidden="1">
+      <c r="A40" s="3"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="71"/>
+      <c r="C40" s="57"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="E40" s="68"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:13" hidden="1">
-      <c r="A41" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10" t="s">
-        <v>59</v>
-      </c>
+    <row r="41" spans="1:12" hidden="1">
+      <c r="A41" s="67"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:13" hidden="1">
-      <c r="A42" s="3" t="s">
-        <v>89</v>
-      </c>
+    <row r="42" spans="1:12" hidden="1">
+      <c r="A42" s="3"/>
       <c r="B42" s="12"/>
-      <c r="C42" s="71"/>
+      <c r="C42" s="57"/>
       <c r="D42" s="12"/>
-      <c r="E42" s="12" t="s">
-        <v>93</v>
-      </c>
+      <c r="E42" s="12"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="10" t="s">
-        <v>100</v>
-      </c>
+      <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:13" hidden="1">
-      <c r="A43" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="71"/>
+    <row r="43" spans="1:12" hidden="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="57"/>
       <c r="D43" s="12"/>
-      <c r="E43" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="E43" s="12"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="G43" s="10"/>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:13" hidden="1">
-      <c r="A44" s="3" t="s">
-        <v>91</v>
-      </c>
+    <row r="44" spans="1:12" hidden="1">
+      <c r="A44" s="3"/>
       <c r="B44" s="10"/>
-      <c r="C44" s="71"/>
+      <c r="C44" s="57"/>
       <c r="D44" s="12"/>
-      <c r="E44" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="E44" s="12"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="10" t="s">
-        <v>98</v>
-      </c>
+      <c r="G44" s="10"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:13" hidden="1">
-      <c r="A45" s="3" t="s">
-        <v>92</v>
-      </c>
+    <row r="45" spans="1:12" hidden="1">
+      <c r="A45" s="3"/>
       <c r="B45" s="10"/>
-      <c r="C45" s="71"/>
+      <c r="C45" s="57"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="E45" s="12"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="G45" s="10"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:13" hidden="1">
+    <row r="46" spans="1:12" hidden="1">
       <c r="A46" s="3"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="71"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="10"/>
@@ -4790,841 +4304,834 @@
       <c r="K46" s="10"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:13" ht="15" hidden="1" thickBot="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="4"/>
-    </row>
-    <row r="48" spans="1:13" ht="15.6" hidden="1" thickTop="1" thickBot="1">
-      <c r="A48" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="18"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="25"/>
-    </row>
-    <row r="49" spans="1:14" ht="101.4" hidden="1" thickTop="1">
-      <c r="A49" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K49" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L49" s="30"/>
-    </row>
-    <row r="50" spans="1:14" hidden="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10">
-        <v>12</v>
-      </c>
-      <c r="K50" s="10"/>
-      <c r="L50" s="4"/>
-    </row>
-    <row r="51" spans="1:14" hidden="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:14" hidden="1">
-      <c r="A52" s="83"/>
-      <c r="B52" s="86"/>
-      <c r="C52" s="85"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="4"/>
-    </row>
-    <row r="53" spans="1:14" hidden="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="71"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-      <c r="L53" s="4"/>
-    </row>
-    <row r="54" spans="1:14" hidden="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="71"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
+    <row r="47" spans="1:12" ht="15" hidden="1" thickBot="1">
+      <c r="A47" s="5"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="6"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" thickTop="1"/>
+    <row r="50" spans="1:14" ht="15" thickBot="1">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50" s="61"/>
+      <c r="D50"/>
+      <c r="E50" s="42"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A51" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="62"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="47"/>
+      <c r="L51"/>
+    </row>
+    <row r="52" spans="1:14" ht="15" thickTop="1">
+      <c r="A52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="48"/>
+      <c r="L52"/>
+    </row>
+    <row r="53" spans="1:14" ht="28.8">
+      <c r="A53" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" s="43"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="M53" s="86" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="28.8">
+      <c r="A54" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E54" s="30"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
-      <c r="L54" s="4"/>
-    </row>
-    <row r="55" spans="1:14" hidden="1">
-      <c r="A55" s="3"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="71"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="85"/>
+      <c r="M54" s="86"/>
+    </row>
+    <row r="55" spans="1:14" ht="43.2">
+      <c r="A55" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="30"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="4"/>
-    </row>
-    <row r="56" spans="1:14" hidden="1">
-      <c r="A56" s="3"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="71"/>
+      <c r="J55" s="90"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="91"/>
+      <c r="M55" s="18"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="64">
+        <v>6</v>
+      </c>
       <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="45"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="4"/>
-    </row>
-    <row r="57" spans="1:14" hidden="1">
-      <c r="A57" s="3"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="71"/>
+      <c r="J56"/>
+      <c r="K56" s="50"/>
+      <c r="L56"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="65">
+        <v>7</v>
+      </c>
       <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="10"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="14"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="4"/>
-    </row>
-    <row r="58" spans="1:14" ht="15" hidden="1" thickBot="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="1:14" ht="15" thickTop="1"/>
-    <row r="61" spans="1:14" ht="15" thickBot="1">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61" s="75"/>
-      <c r="D61"/>
-      <c r="E61" s="53"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
+      <c r="K57" s="50"/>
+      <c r="L57"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="65">
+        <v>0</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="50"/>
+      <c r="L58"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="57">
+        <v>2</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="50"/>
+      <c r="L59"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="57">
+        <v>3</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="37"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="57">
+        <v>1</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="50"/>
       <c r="L61"/>
-      <c r="M61"/>
-      <c r="N61"/>
-    </row>
-    <row r="62" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A62" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="58"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="57">
+        <v>8</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="50"/>
       <c r="L62"/>
     </row>
-    <row r="63" spans="1:14" ht="15" thickTop="1">
-      <c r="A63" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G63" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="59"/>
+    <row r="63" spans="1:14">
+      <c r="A63" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="50"/>
       <c r="L63"/>
-    </row>
-    <row r="64" spans="1:14" ht="28.8">
-      <c r="A64" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="54"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="45"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="45"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="60"/>
-      <c r="L64" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="M64" s="117" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="28.8">
-      <c r="A65" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="78" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E65" s="34"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="61"/>
-      <c r="L65" s="116"/>
-      <c r="M65" s="117"/>
-    </row>
-    <row r="66" spans="1:15">
-      <c r="A66" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C66" s="78">
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="35"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="50"/>
+      <c r="L64"/>
+    </row>
+    <row r="65" spans="1:15" ht="15.6">
+      <c r="A65" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="57">
         <v>1</v>
       </c>
-      <c r="D66" s="50"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="51"/>
-      <c r="K66" s="61"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="10"/>
+      <c r="H65" s="73"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="50"/>
+      <c r="L65"/>
+    </row>
+    <row r="66" spans="1:15" ht="16.2" thickBot="1">
+      <c r="A66" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="57">
+        <v>2</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="46"/>
+      <c r="H66" s="73"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="50"/>
       <c r="L66"/>
     </row>
-    <row r="67" spans="1:15">
-      <c r="A67" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="79">
-        <v>2</v>
-      </c>
-      <c r="D67" s="50"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="61"/>
+    <row r="67" spans="1:15" ht="15.6">
+      <c r="A67" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="10"/>
+      <c r="E67" s="34"/>
+      <c r="H67" s="73"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="50"/>
       <c r="L67"/>
-    </row>
-    <row r="68" spans="1:15">
-      <c r="A68" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="43" t="s">
+      <c r="M67" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="N67" s="76"/>
+      <c r="O67" s="77"/>
+    </row>
+    <row r="68" spans="1:15" ht="15.6">
+      <c r="A68" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="57">
+        <v>4</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="44"/>
+      <c r="H68" s="73"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="50"/>
+      <c r="L68"/>
+      <c r="M68" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N68" s="10"/>
+      <c r="O68" s="79"/>
+    </row>
+    <row r="69" spans="1:15" ht="15.6">
+      <c r="A69" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" s="57">
+        <v>5</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="44"/>
+      <c r="H69" s="73"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="50"/>
+      <c r="L69"/>
+      <c r="M69" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="N69" s="10"/>
+      <c r="O69" s="79"/>
+    </row>
+    <row r="70" spans="1:15" ht="15.6">
+      <c r="A70" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="57">
+        <v>6</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="H70" s="73"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="50"/>
+      <c r="L70"/>
+      <c r="M70" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="N70" s="10"/>
+      <c r="O70" s="79"/>
+    </row>
+    <row r="71" spans="1:15" ht="15.6">
+      <c r="A71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="57">
+        <v>7</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" s="30"/>
+      <c r="H71" s="73"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="50"/>
+      <c r="L71"/>
+      <c r="M71" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="N71" s="10"/>
+      <c r="O71" s="79"/>
+    </row>
+    <row r="72" spans="1:15" ht="15.6">
+      <c r="A72" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="57">
+        <v>8</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="H72" s="73"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="50"/>
+      <c r="L72"/>
+      <c r="M72" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="N72" s="10"/>
+      <c r="O72" s="79"/>
+    </row>
+    <row r="73" spans="1:15" ht="15.6">
+      <c r="A73" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C68" s="79">
+      <c r="C73" s="57">
+        <v>9</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="H73" s="73"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="50"/>
+      <c r="L73"/>
+      <c r="M73" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="N73" s="10"/>
+      <c r="O73" s="79"/>
+    </row>
+    <row r="74" spans="1:15" ht="15.6">
+      <c r="A74" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="57">
+        <v>10</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="H74" s="73"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="50"/>
+      <c r="L74"/>
+      <c r="M74" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="N74" s="41"/>
+      <c r="O74" s="79"/>
+    </row>
+    <row r="75" spans="1:15" ht="15.6">
+      <c r="A75" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C75" s="57">
+        <v>1</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="50"/>
+      <c r="L75"/>
+      <c r="M75" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="N75" s="10"/>
+      <c r="O75" s="79"/>
+    </row>
+    <row r="76" spans="1:15" ht="15.6">
+      <c r="A76" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="57">
         <v>3</v>
       </c>
-      <c r="D68" s="50"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="61"/>
-      <c r="L68"/>
-    </row>
-    <row r="69" spans="1:15">
-      <c r="A69" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="C69" s="80">
-        <v>4</v>
-      </c>
-      <c r="D69" s="50"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="61"/>
-      <c r="L69"/>
-    </row>
-    <row r="70" spans="1:15">
-      <c r="A70" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="80">
-        <v>5</v>
-      </c>
-      <c r="D70" s="50"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="61"/>
-      <c r="L70" s="44"/>
-    </row>
-    <row r="71" spans="1:15">
-      <c r="A71" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C71" s="80">
-        <v>6</v>
-      </c>
-      <c r="D71" s="50"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="61"/>
-      <c r="L71"/>
-    </row>
-    <row r="72" spans="1:15">
-      <c r="A72" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="80">
-        <v>8</v>
-      </c>
-      <c r="D72" s="50"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="10"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="61"/>
-      <c r="L72"/>
-    </row>
-    <row r="73" spans="1:15">
-      <c r="A73" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" s="43"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="61"/>
-      <c r="L73"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-    </row>
-    <row r="74" spans="1:15">
-      <c r="A74" s="41"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="61"/>
-      <c r="L74"/>
-    </row>
-    <row r="75" spans="1:15" ht="15.6">
-      <c r="A75" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C75" s="80">
-        <v>1</v>
-      </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="39"/>
-      <c r="H75" s="90"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="39"/>
-      <c r="K75" s="61"/>
-      <c r="L75"/>
-    </row>
-    <row r="76" spans="1:15" ht="16.2" thickBot="1">
-      <c r="A76" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="71">
-        <v>2</v>
-      </c>
-      <c r="D76" s="39"/>
-      <c r="E76" s="57"/>
-      <c r="H76" s="90"/>
-      <c r="I76" s="39"/>
-      <c r="J76" s="39"/>
-      <c r="K76" s="61"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="50"/>
       <c r="L76"/>
+      <c r="M76" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="N76" s="10"/>
+      <c r="O76" s="79"/>
     </row>
     <row r="77" spans="1:15" ht="15.6">
-      <c r="A77" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" s="39"/>
-      <c r="C77" s="80">
-        <v>3</v>
-      </c>
-      <c r="D77" s="39"/>
-      <c r="E77" s="38"/>
-      <c r="H77" s="90"/>
-      <c r="I77" s="39"/>
-      <c r="J77" s="39"/>
-      <c r="K77" s="61"/>
+      <c r="A77" s="35"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="50"/>
       <c r="L77"/>
-      <c r="M77" s="92" t="s">
-        <v>158</v>
-      </c>
-      <c r="N77" s="93"/>
-      <c r="O77" s="94"/>
-    </row>
-    <row r="78" spans="1:15" ht="15.6">
-      <c r="A78" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" s="71">
-        <v>4</v>
-      </c>
-      <c r="D78" s="39"/>
-      <c r="E78" s="55"/>
-      <c r="H78" s="90"/>
-      <c r="I78" s="39"/>
-      <c r="J78" s="39"/>
-      <c r="K78" s="61"/>
+      <c r="M77" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="O77" s="79"/>
+    </row>
+    <row r="78" spans="1:15" ht="15" thickBot="1">
+      <c r="A78" s="35"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="57"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="50"/>
       <c r="L78"/>
-      <c r="M78" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="N78" s="39"/>
-      <c r="O78" s="96"/>
-    </row>
-    <row r="79" spans="1:15" ht="15.6">
-      <c r="A79" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C79" s="71">
-        <v>5</v>
-      </c>
-      <c r="D79" s="39"/>
-      <c r="E79" s="55"/>
-      <c r="H79" s="90"/>
-      <c r="I79" s="39"/>
-      <c r="J79" s="39"/>
-      <c r="K79" s="61"/>
+      <c r="M78" s="80"/>
+      <c r="N78" s="81"/>
+      <c r="O78" s="82"/>
+    </row>
+    <row r="79" spans="1:15" ht="15" thickBot="1">
+      <c r="A79" s="40"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="51"/>
       <c r="L79"/>
-      <c r="M79" s="95" t="s">
-        <v>138</v>
-      </c>
-      <c r="N79" s="39"/>
-      <c r="O79" s="96"/>
-    </row>
-    <row r="80" spans="1:15" ht="15.6">
-      <c r="A80" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B80" s="91" t="s">
-        <v>150</v>
-      </c>
-      <c r="C80" s="71">
-        <v>6</v>
-      </c>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="H80" s="90"/>
-      <c r="I80" s="39"/>
-      <c r="J80" s="39"/>
-      <c r="K80" s="61"/>
-      <c r="L80"/>
-      <c r="M80" s="95" t="s">
-        <v>139</v>
-      </c>
-      <c r="N80" s="39"/>
-      <c r="O80" s="96"/>
-    </row>
-    <row r="81" spans="1:15" ht="15.6">
-      <c r="A81" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="C81" s="71">
-        <v>7</v>
-      </c>
-      <c r="D81" s="39"/>
-      <c r="E81" s="34"/>
-      <c r="H81" s="90"/>
-      <c r="I81" s="39"/>
-      <c r="J81" s="39"/>
-      <c r="K81" s="61"/>
-      <c r="L81"/>
-      <c r="M81" s="95" t="s">
-        <v>140</v>
-      </c>
-      <c r="N81" s="10"/>
-      <c r="O81" s="96"/>
-    </row>
-    <row r="82" spans="1:15" ht="15.6">
-      <c r="A82" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B82" s="91" t="s">
-        <v>152</v>
-      </c>
-      <c r="C82" s="71">
-        <v>8</v>
-      </c>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="H82" s="90"/>
-      <c r="I82" s="39"/>
-      <c r="J82" s="39"/>
-      <c r="K82" s="61"/>
-      <c r="L82"/>
-      <c r="M82" s="95" t="s">
-        <v>141</v>
-      </c>
-      <c r="N82" s="10"/>
-      <c r="O82" s="96"/>
-    </row>
-    <row r="83" spans="1:15" ht="15.6">
-      <c r="A83" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="71">
-        <v>9</v>
-      </c>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="H83" s="90"/>
-      <c r="I83" s="39"/>
-      <c r="J83" s="39"/>
-      <c r="K83" s="61"/>
-      <c r="L83"/>
-      <c r="M83" s="95" t="s">
-        <v>142</v>
-      </c>
-      <c r="N83" s="10"/>
-      <c r="O83" s="96"/>
-    </row>
-    <row r="84" spans="1:15" ht="15.6">
-      <c r="A84" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B84" s="91" t="s">
-        <v>157</v>
-      </c>
-      <c r="C84" s="71">
-        <v>10</v>
-      </c>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="H84" s="90"/>
-      <c r="I84" s="39"/>
-      <c r="J84" s="39"/>
-      <c r="K84" s="61"/>
-      <c r="L84"/>
-      <c r="M84" s="95" t="s">
-        <v>143</v>
-      </c>
-      <c r="N84" s="52"/>
-      <c r="O84" s="96"/>
-    </row>
-    <row r="85" spans="1:15" ht="15.6">
-      <c r="A85" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" s="91" t="s">
-        <v>147</v>
-      </c>
-      <c r="C85" s="71">
-        <v>1</v>
-      </c>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="H85" s="39"/>
-      <c r="I85" s="39"/>
-      <c r="J85" s="39"/>
-      <c r="K85" s="61"/>
-      <c r="L85"/>
-      <c r="M85" s="95" t="s">
-        <v>144</v>
-      </c>
-      <c r="N85" s="39"/>
-      <c r="O85" s="96"/>
-    </row>
-    <row r="86" spans="1:15" ht="15.6">
-      <c r="A86" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B86" s="91" t="s">
-        <v>148</v>
-      </c>
-      <c r="C86" s="71">
-        <v>3</v>
-      </c>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="H86" s="39"/>
-      <c r="I86" s="39"/>
-      <c r="J86" s="39"/>
-      <c r="K86" s="61"/>
+    </row>
+    <row r="80" spans="1:15" ht="15" thickTop="1">
+      <c r="A80" s="2"/>
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="E81" s="18"/>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="E82" s="18"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="E83" s="18"/>
+      <c r="K83" s="1"/>
+      <c r="N83"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="E84" s="18"/>
+      <c r="K84" s="1"/>
+      <c r="N84"/>
+    </row>
+    <row r="85" spans="1:14">
+      <c r="E85" s="18"/>
+      <c r="K85" s="1"/>
+      <c r="N85"/>
+    </row>
+    <row r="86" spans="1:14">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86" s="61"/>
+      <c r="D86"/>
+      <c r="E86" s="42"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
       <c r="L86"/>
-      <c r="M86" s="95" t="s">
-        <v>145</v>
-      </c>
-      <c r="N86" s="39"/>
-      <c r="O86" s="96"/>
-    </row>
-    <row r="87" spans="1:15" ht="15.6">
-      <c r="A87" s="41"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="80"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="H87" s="39"/>
-      <c r="I87" s="39"/>
-      <c r="J87" s="39"/>
-      <c r="K87" s="61"/>
+      <c r="M86"/>
+      <c r="N86"/>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87" s="61"/>
+      <c r="D87"/>
+      <c r="E87" s="42"/>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
       <c r="L87"/>
-      <c r="M87" s="95" t="s">
-        <v>146</v>
-      </c>
-      <c r="N87" s="65"/>
-      <c r="O87" s="96"/>
-    </row>
-    <row r="88" spans="1:15" ht="15" thickBot="1">
-      <c r="A88" s="41"/>
-      <c r="B88" s="43"/>
-      <c r="C88" s="80"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="39"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="39"/>
-      <c r="J88" s="39"/>
-      <c r="K88" s="61"/>
+      <c r="M87"/>
+      <c r="N87"/>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88" s="61"/>
+      <c r="D88"/>
+      <c r="E88" s="42"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+      <c r="K88"/>
       <c r="L88"/>
-      <c r="M88" s="97"/>
-      <c r="N88" s="98"/>
-      <c r="O88" s="99"/>
-    </row>
-    <row r="89" spans="1:15" ht="15" thickBot="1">
-      <c r="A89" s="47"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="81"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="40"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="40"/>
-      <c r="H89" s="40"/>
-      <c r="I89" s="40"/>
-      <c r="J89" s="40"/>
-      <c r="K89" s="62"/>
+      <c r="M88"/>
+      <c r="N88"/>
+    </row>
+    <row r="89" spans="1:14">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89" s="61"/>
+      <c r="D89"/>
+      <c r="E89" s="42"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
       <c r="L89"/>
-    </row>
-    <row r="90" spans="1:15" ht="15" thickTop="1">
-      <c r="A90" s="2"/>
-      <c r="D90" s="1"/>
-      <c r="K90" s="64"/>
-    </row>
-    <row r="91" spans="1:15">
-      <c r="A91" s="65"/>
-      <c r="B91" s="65"/>
-      <c r="C91" s="82"/>
-      <c r="D91" s="67"/>
-      <c r="E91" s="67"/>
-      <c r="F91" s="65"/>
-      <c r="G91" s="65"/>
-      <c r="H91" s="65"/>
-      <c r="I91" s="65"/>
-      <c r="K91" s="65"/>
-      <c r="L91" s="65"/>
-    </row>
-    <row r="92" spans="1:15">
-      <c r="A92" s="65"/>
-      <c r="B92" s="65"/>
-      <c r="C92" s="82"/>
-      <c r="D92" s="67"/>
-      <c r="E92" s="67"/>
-      <c r="F92" s="65"/>
-      <c r="G92" s="65"/>
-      <c r="H92" s="65"/>
-      <c r="I92" s="65"/>
-      <c r="J92" s="65"/>
-      <c r="K92" s="65"/>
-      <c r="L92" s="65"/>
-    </row>
-    <row r="93" spans="1:15">
-      <c r="D93" s="64"/>
-      <c r="E93" s="64"/>
-      <c r="K93" s="1"/>
+      <c r="M89"/>
+      <c r="N89"/>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90" s="61"/>
+      <c r="D90"/>
+      <c r="E90" s="42"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+      <c r="N90"/>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91" s="61"/>
+      <c r="D91"/>
+      <c r="E91" s="42"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+    </row>
+    <row r="92" spans="1:14">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92" s="61"/>
+      <c r="D92"/>
+      <c r="E92" s="42"/>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+      <c r="N92"/>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93" s="61"/>
+      <c r="D93"/>
+      <c r="E93" s="42"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:15">
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="K94" s="1"/>
+    <row r="94" spans="1:14">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94" s="61"/>
+      <c r="D94"/>
+      <c r="E94" s="42"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:15">
-      <c r="D95" s="64"/>
-      <c r="E95" s="64"/>
-      <c r="K95" s="1"/>
+    <row r="95" spans="1:14">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95" s="61"/>
+      <c r="D95"/>
+      <c r="E95" s="42"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:14">
       <c r="A96"/>
       <c r="B96"/>
-      <c r="C96" s="75"/>
+      <c r="C96" s="61"/>
       <c r="D96"/>
-      <c r="E96" s="53"/>
+      <c r="E96" s="42"/>
       <c r="F96"/>
       <c r="G96"/>
       <c r="H96"/>
@@ -5638,9 +5145,9 @@
     <row r="97" spans="1:14">
       <c r="A97"/>
       <c r="B97"/>
-      <c r="C97" s="75"/>
+      <c r="C97" s="61"/>
       <c r="D97"/>
-      <c r="E97" s="53"/>
+      <c r="E97" s="42"/>
       <c r="F97"/>
       <c r="G97"/>
       <c r="H97"/>
@@ -5651,180 +5158,20 @@
       <c r="M97"/>
       <c r="N97"/>
     </row>
-    <row r="98" spans="1:14">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98" s="75"/>
-      <c r="D98"/>
-      <c r="E98" s="53"/>
-      <c r="F98"/>
-      <c r="G98"/>
-      <c r="H98"/>
-      <c r="I98"/>
-      <c r="J98"/>
-      <c r="K98"/>
-      <c r="L98"/>
-      <c r="M98"/>
-      <c r="N98"/>
-    </row>
     <row r="99" spans="1:14">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99" s="75"/>
-      <c r="D99"/>
-      <c r="E99" s="53"/>
-      <c r="F99"/>
-      <c r="G99"/>
-      <c r="H99"/>
-      <c r="I99"/>
-      <c r="J99"/>
-      <c r="K99"/>
-      <c r="L99"/>
-      <c r="M99"/>
-      <c r="N99"/>
+      <c r="A99" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="100" spans="1:14">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100" s="75"/>
-      <c r="D100"/>
-      <c r="E100" s="53"/>
-      <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="L100"/>
-      <c r="M100"/>
-      <c r="N100"/>
-    </row>
-    <row r="101" spans="1:14">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101" s="75"/>
-      <c r="D101"/>
-      <c r="E101" s="53"/>
-      <c r="F101"/>
-      <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
-      <c r="J101"/>
-      <c r="K101"/>
-      <c r="L101"/>
-      <c r="M101"/>
-      <c r="N101"/>
-    </row>
-    <row r="102" spans="1:14">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102" s="75"/>
-      <c r="D102"/>
-      <c r="E102" s="53"/>
-      <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-      <c r="J102"/>
-      <c r="K102"/>
-      <c r="L102"/>
-      <c r="M102"/>
-      <c r="N102"/>
-    </row>
-    <row r="103" spans="1:14">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103" s="75"/>
-      <c r="D103"/>
-      <c r="E103" s="53"/>
-      <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="L103"/>
-      <c r="M103"/>
-      <c r="N103"/>
-    </row>
-    <row r="104" spans="1:14">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104" s="75"/>
-      <c r="D104"/>
-      <c r="E104" s="53"/>
-      <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104"/>
-      <c r="M104"/>
-      <c r="N104"/>
-    </row>
-    <row r="105" spans="1:14">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105" s="75"/>
-      <c r="D105"/>
-      <c r="E105" s="53"/>
-      <c r="F105"/>
-      <c r="G105"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
-    </row>
-    <row r="106" spans="1:14">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106" s="75"/>
-      <c r="D106"/>
-      <c r="E106" s="53"/>
-      <c r="F106"/>
-      <c r="G106"/>
-      <c r="H106"/>
-      <c r="I106"/>
-      <c r="J106"/>
-      <c r="K106"/>
-      <c r="L106"/>
-      <c r="M106"/>
-      <c r="N106"/>
-    </row>
-    <row r="107" spans="1:14">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107" s="75"/>
-      <c r="D107"/>
-      <c r="E107" s="53"/>
-      <c r="F107"/>
-      <c r="G107"/>
-      <c r="H107"/>
-      <c r="I107"/>
-      <c r="J107"/>
-      <c r="K107"/>
-      <c r="L107"/>
-      <c r="M107"/>
-      <c r="N107"/>
-    </row>
-    <row r="109" spans="1:14">
-      <c r="A109" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14">
-      <c r="A110" s="2" t="s">
-        <v>87</v>
+      <c r="A100" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L64:L65"/>
-    <mergeCell ref="M64:M65"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="M53:M54"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.45" right="0.45" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
@@ -5833,7 +5180,7 @@
     <oddFooter>&amp;R&amp;8&amp;F</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="58" max="16383" man="1"/>
+    <brk id="47" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the drive motor colors
</commit_message>
<xml_diff>
--- a/documentations/2023 coordination sheet.xlsx
+++ b/documentations/2023 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2023-prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70119DC-E32A-4DAD-91B1-572AF70C548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065A72DD-6F02-46B7-B06B-EAE036CDE315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -806,9 +806,6 @@
     <t>PDP 18</t>
   </si>
   <si>
-    <t>Orange</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -846,6 +843,9 @@
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1702,35 +1702,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3373,7 +3361,7 @@
   <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3469,7 +3457,7 @@
         <v>56</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>158</v>
@@ -3510,7 +3498,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>70</v>
@@ -3551,7 +3539,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>150</v>
@@ -3590,7 +3578,7 @@
         <v>61</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>26</v>
@@ -3610,19 +3598,8 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="91"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
+      <c r="D9" s="83"/>
+      <c r="I9" s="88"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1">
       <c r="D10" s="83"/>
@@ -4339,8 +4316,8 @@
       <c r="A51" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="87" t="s">
-        <v>161</v>
+      <c r="B51" s="85" t="s">
+        <v>160</v>
       </c>
       <c r="C51" s="62"/>
       <c r="D51" s="25"/>
@@ -4387,14 +4364,14 @@
       <c r="A53" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="88" t="s">
-        <v>162</v>
+      <c r="B53" s="86" t="s">
+        <v>161</v>
       </c>
       <c r="C53" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D53" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="38"/>
@@ -4403,10 +4380,10 @@
       <c r="I53" s="38"/>
       <c r="J53" s="38"/>
       <c r="K53" s="49"/>
-      <c r="L53" s="85" t="s">
+      <c r="L53" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="M53" s="86" t="s">
+      <c r="M53" s="90" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4414,14 +4391,14 @@
       <c r="A54" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="89" t="s">
-        <v>163</v>
+      <c r="B54" s="87" t="s">
+        <v>162</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E54" s="30"/>
       <c r="F54" s="10"/>
@@ -4430,30 +4407,29 @@
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="50"/>
-      <c r="L54" s="85"/>
-      <c r="M54" s="86"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="90"/>
     </row>
     <row r="55" spans="1:14" ht="43.2">
       <c r="A55" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="89" t="s">
+      <c r="B55" s="87" t="s">
         <v>40</v>
       </c>
       <c r="C55" s="64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E55" s="30"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
-      <c r="J55" s="90"/>
       <c r="K55" s="50"/>
-      <c r="L55" s="91"/>
+      <c r="L55" s="18"/>
       <c r="M55" s="18"/>
     </row>
     <row r="56" spans="1:14">
@@ -4669,10 +4645,10 @@
         <v>69</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="57" t="s">
         <v>169</v>
-      </c>
-      <c r="C67" s="57" t="s">
-        <v>170</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="34"/>

</xml_diff>

<commit_message>
updated coord sheet. balance does not work for new chassis and i dont know why :(((((
</commit_message>
<xml_diff>
--- a/documentations/2023 coordination sheet.xlsx
+++ b/documentations/2023 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2023-prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D0F975-30C1-4B0F-82FC-1D95A75DA732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C333BF-E660-44AB-A838-604969D29B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,7 +851,7 @@
     <t>Talon</t>
   </si>
   <si>
-    <t>ID-8</t>
+    <t>ID-6</t>
   </si>
 </sst>
 </file>
@@ -3367,7 +3367,7 @@
   <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3463,7 +3463,7 @@
         <v>56</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>158</v>
@@ -3504,7 +3504,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>70</v>
@@ -3545,7 +3545,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>150</v>
@@ -3584,7 +3584,7 @@
         <v>61</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated coord sheet with motor colors
</commit_message>
<xml_diff>
--- a/documentations/2023 coordination sheet.xlsx
+++ b/documentations/2023 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2023-prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C333BF-E660-44AB-A838-604969D29B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABD74E3-A9D5-460D-973C-C56FA5D86B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
   <si>
     <t>Relay Function Chart</t>
   </si>
@@ -852,6 +852,36 @@
   </si>
   <si>
     <t>ID-6</t>
+  </si>
+  <si>
+    <t>Wrist motor</t>
+  </si>
+  <si>
+    <t>talon</t>
+  </si>
+  <si>
+    <t>ID-14</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Joust Motor</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Turret Motor</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Arm Pivot</t>
   </si>
 </sst>
 </file>
@@ -1756,14 +1786,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>417635</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>3395</xdr:rowOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>3396</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1799,13 +1829,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1821,7 +1851,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12152049" y="8238386"/>
+          <a:off x="12152049" y="8978192"/>
           <a:ext cx="1778957" cy="1674088"/>
           <a:chOff x="10410824" y="9220200"/>
           <a:chExt cx="1771651" cy="1933575"/>
@@ -2806,13 +2836,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>64156</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>143059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>74490</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>92772</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3364,10 +3394,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3613,180 +3643,132 @@
       </c>
       <c r="I9" s="88"/>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="C10" s="55" t="s">
+        <v>21</v>
+      </c>
       <c r="D10" s="83"/>
-      <c r="E10" s="28"/>
+      <c r="E10" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="F10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="88"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="83"/>
+      <c r="G11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" s="88"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="83"/>
+      <c r="G12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I12" s="88"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="83"/>
+      <c r="G13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I13" s="88"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1">
+      <c r="A14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="83"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="D11" s="83"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="D15" s="83"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
-      <c r="A13" s="7" t="s">
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E17" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K17" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M17" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="3" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="10" t="s">
+      <c r="C18" s="59"/>
+      <c r="D18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E18" s="24">
         <v>2</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="24">
-        <v>10</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="22"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="24">
-        <v>3</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="24">
-        <v>4</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="22"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="24">
-        <v>5</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="10"/>
@@ -3795,23 +3777,23 @@
       <c r="J18" s="10"/>
       <c r="K18" s="12"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="22"/>
+      <c r="M18" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>139</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D19" s="10"/>
       <c r="E19" s="24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="10"/>
@@ -3824,19 +3806,17 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E20" s="32">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="24">
+        <v>3</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="10"/>
@@ -3845,15 +3825,27 @@
       <c r="J20" s="10"/>
       <c r="K20" s="12"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="22"/>
-    </row>
-    <row r="21" spans="1:13" hidden="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="14"/>
+      <c r="M20" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="24">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -3862,12 +3854,22 @@
       <c r="L21" s="10"/>
       <c r="M21" s="22"/>
     </row>
-    <row r="22" spans="1:13" hidden="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="24"/>
+    <row r="22" spans="1:13">
+      <c r="A22" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="24">
+        <v>5</v>
+      </c>
       <c r="F22" s="14"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -3879,19 +3881,19 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E23" s="24">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="10"/>
@@ -3904,19 +3906,19 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C24" s="59" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="24">
-        <v>8</v>
+        <v>140</v>
+      </c>
+      <c r="E24" s="32">
+        <v>7</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="10"/>
@@ -3927,167 +3929,167 @@
       <c r="L24" s="10"/>
       <c r="M24" s="22"/>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:13" hidden="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="26" spans="1:13" hidden="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="22"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="24">
+        <v>11</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="22"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="24">
+        <v>8</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="22"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickBot="1">
+      <c r="A29" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C29" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E29" s="23">
         <v>9</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="23"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" hidden="1" thickTop="1">
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" hidden="1" thickBot="1">
-      <c r="A27" s="2" t="s">
+      <c r="F29" s="15"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="23"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" hidden="1" thickTop="1">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" hidden="1" thickBot="1">
+      <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="18"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="28"/>
-    </row>
-    <row r="28" spans="1:13" ht="84.6" hidden="1" thickTop="1">
-      <c r="A28" s="20" t="s">
+      <c r="E31" s="18"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" spans="1:13" ht="84.6" hidden="1" thickTop="1">
+      <c r="A32" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C32" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9" t="s">
+      <c r="F32" s="8"/>
+      <c r="G32" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="26" t="s">
+      <c r="H32" s="9"/>
+      <c r="I32" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K32" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L28" s="29"/>
-    </row>
-    <row r="29" spans="1:13" hidden="1">
-      <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:13" hidden="1">
-      <c r="A30" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" hidden="1">
-      <c r="A31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" hidden="1">
-      <c r="A32" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="4"/>
+      <c r="L32" s="29"/>
     </row>
     <row r="33" spans="1:12" hidden="1">
       <c r="A33" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="B33" s="12"/>
       <c r="C33" s="57"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -4097,17 +4099,17 @@
     </row>
     <row r="34" spans="1:12" hidden="1">
       <c r="A34" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="B34" s="12"/>
       <c r="C34" s="57"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
@@ -4116,155 +4118,179 @@
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" hidden="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="12"/>
       <c r="C35" s="57"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" ht="15" hidden="1" thickBot="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="10"/>
+    <row r="36" spans="1:12" hidden="1">
+      <c r="A36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="12"/>
       <c r="C36" s="57"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" ht="15.6" hidden="1" thickTop="1" thickBot="1">
-      <c r="A37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="18"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="25"/>
-    </row>
-    <row r="38" spans="1:12" ht="101.4" hidden="1" thickTop="1">
-      <c r="A38" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="9"/>
-      <c r="I38" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L38" s="29"/>
+    <row r="37" spans="1:12" hidden="1">
+      <c r="A37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" hidden="1">
+      <c r="A38" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" hidden="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="12"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="57"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
-      <c r="J39" s="10">
-        <v>12</v>
-      </c>
+      <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12" ht="15" hidden="1" thickBot="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="12"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="57"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:12" hidden="1">
-      <c r="A41" s="67"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="4"/>
-    </row>
-    <row r="42" spans="1:12" hidden="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="4"/>
+    <row r="41" spans="1:12" ht="15.6" hidden="1" thickTop="1" thickBot="1">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="25"/>
+    </row>
+    <row r="42" spans="1:12" ht="101.4" hidden="1" thickTop="1">
+      <c r="A42" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="29"/>
     </row>
     <row r="43" spans="1:12" hidden="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="10"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="57"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
+      <c r="J43" s="10">
+        <v>12</v>
+      </c>
       <c r="K43" s="10"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" hidden="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="10"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="57"/>
       <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
@@ -4272,13 +4298,13 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:12" hidden="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -4287,7 +4313,7 @@
     </row>
     <row r="46" spans="1:12" hidden="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="10"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="57"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
@@ -4299,270 +4325,246 @@
       <c r="K46" s="10"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" ht="15" hidden="1" thickBot="1">
-      <c r="A47" s="5"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" thickTop="1"/>
-    <row r="50" spans="1:14" ht="15" thickBot="1">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50" s="61"/>
-      <c r="D50"/>
-      <c r="E50" s="42"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-    </row>
-    <row r="51" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A51" s="36" t="s">
+    <row r="47" spans="1:12" hidden="1">
+      <c r="A47" s="3"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="1:12" hidden="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:14" hidden="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="1:14" hidden="1">
+      <c r="A50" s="3"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:14" ht="15" hidden="1" thickBot="1">
+      <c r="A51" s="5"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="1:14" ht="15" thickTop="1"/>
+    <row r="54" spans="1:14" ht="15" thickBot="1">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54" s="61"/>
+      <c r="D54"/>
+      <c r="E54" s="42"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A55" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="85" t="s">
+      <c r="B55" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="62"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="47"/>
-      <c r="L51"/>
-    </row>
-    <row r="52" spans="1:14" ht="15" thickTop="1">
-      <c r="A52" s="8" t="s">
+      <c r="C55" s="62"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="47"/>
+      <c r="L55"/>
+    </row>
+    <row r="56" spans="1:14" ht="15" thickTop="1">
+      <c r="A56" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="54" t="s">
+      <c r="C56" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F56" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G52" s="39" t="s">
+      <c r="G56" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H56" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="48"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:14" ht="28.8">
-      <c r="A53" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="86" t="s">
-        <v>161</v>
-      </c>
-      <c r="C53" s="63" t="s">
-        <v>163</v>
-      </c>
-      <c r="D53" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="E53" s="43"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="89" t="s">
-        <v>67</v>
-      </c>
-      <c r="M53" s="90" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="28.8">
-      <c r="A54" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" s="87" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E54" s="30"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="50"/>
-      <c r="L54" s="89"/>
-      <c r="M54" s="90"/>
-    </row>
-    <row r="55" spans="1:14" ht="43.2">
-      <c r="A55" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="87" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" s="30"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="64">
-        <v>6</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56"/>
-      <c r="K56" s="50"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="48"/>
       <c r="L56"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" ht="28.8">
       <c r="A57" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="65">
-        <v>7</v>
-      </c>
-      <c r="D57" s="12"/>
+      <c r="B57" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>166</v>
+      </c>
       <c r="E57" s="43"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="50"/>
-      <c r="L57"/>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="M57" s="90" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="28.8">
       <c r="A58" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" s="65">
-        <v>0</v>
-      </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="14"/>
+      <c r="B58" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" s="30"/>
+      <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
       <c r="K58" s="50"/>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="L58" s="89"/>
+      <c r="M58" s="90"/>
+    </row>
+    <row r="59" spans="1:14" ht="43.2">
       <c r="A59" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" s="57">
-        <v>2</v>
-      </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="43"/>
+      <c r="B59" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="30"/>
       <c r="F59" s="14"/>
-      <c r="G59" s="10"/>
+      <c r="G59" s="14"/>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
-      <c r="J59" s="10"/>
       <c r="K59" s="50"/>
-      <c r="L59"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="57">
-        <v>3</v>
+        <v>66</v>
+      </c>
+      <c r="C60" s="64">
+        <v>6</v>
       </c>
       <c r="D60" s="12"/>
-      <c r="E60" s="43"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="14"/>
-      <c r="G60" s="10"/>
+      <c r="G60" s="45"/>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
-      <c r="J60" s="10"/>
+      <c r="J60"/>
       <c r="K60" s="50"/>
-      <c r="L60" s="37"/>
+      <c r="L60"/>
     </row>
     <row r="61" spans="1:14">
       <c r="A61" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="57">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C61" s="65">
+        <v>7</v>
       </c>
       <c r="D61" s="12"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
@@ -4575,14 +4577,14 @@
         <v>65</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="57">
-        <v>8</v>
+        <v>108</v>
+      </c>
+      <c r="C62" s="65">
+        <v>0</v>
       </c>
       <c r="D62" s="12"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
@@ -4594,204 +4596,192 @@
       <c r="A63" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="35"/>
+      <c r="B63" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="57">
+        <v>2</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
       <c r="J63" s="10"/>
       <c r="K63" s="50"/>
       <c r="L63"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="35"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
+      <c r="A64" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="57">
+        <v>3</v>
+      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="14"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
       <c r="J64" s="10"/>
       <c r="K64" s="50"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" spans="1:15" ht="15.6">
+      <c r="L64" s="37"/>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>129</v>
+        <v>65</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="C65" s="57">
         <v>1</v>
       </c>
-      <c r="D65" s="30"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="10"/>
-      <c r="H65" s="73"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
       <c r="K65" s="50"/>
       <c r="L65"/>
     </row>
-    <row r="66" spans="1:15" ht="16.2" thickBot="1">
+    <row r="66" spans="1:15">
       <c r="A66" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>131</v>
+        <v>65</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="C66" s="57">
-        <v>2</v>
-      </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="46"/>
-      <c r="H66" s="73"/>
+        <v>8</v>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10"/>
       <c r="K66" s="50"/>
       <c r="L66"/>
     </row>
-    <row r="67" spans="1:15" ht="15.6">
+    <row r="67" spans="1:15">
       <c r="A67" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C67" s="57" t="s">
-        <v>169</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="57"/>
       <c r="D67" s="10"/>
-      <c r="E67" s="34"/>
-      <c r="H67" s="73"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="10"/>
       <c r="K67" s="50"/>
       <c r="L67"/>
-      <c r="M67" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="N67" s="76"/>
-      <c r="O67" s="77"/>
-    </row>
-    <row r="68" spans="1:15" ht="15.6">
-      <c r="A68" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C68" s="57">
-        <v>4</v>
-      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="A68" s="35"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="57"/>
       <c r="D68" s="10"/>
-      <c r="E68" s="44"/>
-      <c r="H68" s="73"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
       <c r="I68" s="10"/>
       <c r="J68" s="10"/>
       <c r="K68" s="50"/>
       <c r="L68"/>
-      <c r="M68" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="N68" s="10"/>
-      <c r="O68" s="79"/>
     </row>
     <row r="69" spans="1:15" ht="15.6">
       <c r="A69" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C69" s="57">
-        <v>5</v>
-      </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="30"/>
+      <c r="E69" s="10"/>
       <c r="H69" s="73"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
       <c r="K69" s="50"/>
       <c r="L69"/>
-      <c r="M69" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="N69" s="10"/>
-      <c r="O69" s="79"/>
-    </row>
-    <row r="70" spans="1:15" ht="15.6">
+    </row>
+    <row r="70" spans="1:15" ht="16.2" thickBot="1">
       <c r="A70" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="74" t="s">
-        <v>126</v>
+      <c r="B70" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C70" s="57">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
+      <c r="E70" s="46"/>
       <c r="H70" s="73"/>
       <c r="I70" s="10"/>
       <c r="J70" s="10"/>
       <c r="K70" s="50"/>
       <c r="L70"/>
-      <c r="M70" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="N70" s="10"/>
-      <c r="O70" s="79"/>
     </row>
     <row r="71" spans="1:15" ht="15.6">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="C71" s="57">
-        <v>7</v>
+      <c r="B71" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C71" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="D71" s="10"/>
-      <c r="E71" s="30"/>
+      <c r="E71" s="34"/>
       <c r="H71" s="73"/>
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
       <c r="K71" s="50"/>
       <c r="L71"/>
-      <c r="M71" s="78" t="s">
-        <v>116</v>
-      </c>
-      <c r="N71" s="10"/>
-      <c r="O71" s="79"/>
+      <c r="M71" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="N71" s="76"/>
+      <c r="O71" s="77"/>
     </row>
     <row r="72" spans="1:15" ht="15.6">
       <c r="A72" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="74" t="s">
-        <v>128</v>
+      <c r="B72" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="C72" s="57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
+      <c r="E72" s="44"/>
       <c r="H72" s="73"/>
       <c r="I72" s="10"/>
       <c r="J72" s="10"/>
       <c r="K72" s="50"/>
       <c r="L72"/>
       <c r="M72" s="78" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="N72" s="10"/>
       <c r="O72" s="79"/>
@@ -4800,21 +4790,21 @@
       <c r="A73" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="74" t="s">
-        <v>132</v>
+      <c r="B73" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C73" s="57">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
+      <c r="E73" s="44"/>
       <c r="H73" s="73"/>
       <c r="I73" s="10"/>
       <c r="J73" s="10"/>
       <c r="K73" s="50"/>
       <c r="L73"/>
       <c r="M73" s="78" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N73" s="10"/>
       <c r="O73" s="79"/>
@@ -4824,10 +4814,10 @@
         <v>69</v>
       </c>
       <c r="B74" s="74" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C74" s="57">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="10"/>
@@ -4837,30 +4827,30 @@
       <c r="K74" s="50"/>
       <c r="L74"/>
       <c r="M74" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="N74" s="41"/>
+        <v>115</v>
+      </c>
+      <c r="N74" s="10"/>
       <c r="O74" s="79"/>
     </row>
     <row r="75" spans="1:15" ht="15.6">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B75" s="74" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C75" s="57">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="H75" s="10"/>
+      <c r="E75" s="30"/>
+      <c r="H75" s="73"/>
       <c r="I75" s="10"/>
       <c r="J75" s="10"/>
       <c r="K75" s="50"/>
       <c r="L75"/>
       <c r="M75" s="78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N75" s="10"/>
       <c r="O75" s="79"/>
@@ -4870,161 +4860,189 @@
         <v>69</v>
       </c>
       <c r="B76" s="74" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C76" s="57">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
-      <c r="H76" s="10"/>
+      <c r="H76" s="73"/>
       <c r="I76" s="10"/>
       <c r="J76" s="10"/>
       <c r="K76" s="50"/>
       <c r="L76"/>
       <c r="M76" s="78" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="N76" s="10"/>
       <c r="O76" s="79"/>
     </row>
     <row r="77" spans="1:15" ht="15.6">
-      <c r="A77" s="35"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="57"/>
+      <c r="A77" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="57">
+        <v>9</v>
+      </c>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
-      <c r="H77" s="10"/>
+      <c r="H77" s="73"/>
       <c r="I77" s="10"/>
       <c r="J77" s="10"/>
       <c r="K77" s="50"/>
       <c r="L77"/>
       <c r="M77" s="78" t="s">
-        <v>122</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="N77" s="10"/>
       <c r="O77" s="79"/>
     </row>
-    <row r="78" spans="1:15" ht="15" thickBot="1">
-      <c r="A78" s="35"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="57"/>
-      <c r="D78" s="30"/>
+    <row r="78" spans="1:15" ht="15.6">
+      <c r="A78" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78" s="57">
+        <v>10</v>
+      </c>
+      <c r="D78" s="10"/>
       <c r="E78" s="10"/>
-      <c r="H78" s="10"/>
+      <c r="H78" s="73"/>
       <c r="I78" s="10"/>
       <c r="J78" s="10"/>
       <c r="K78" s="50"/>
       <c r="L78"/>
-      <c r="M78" s="80"/>
-      <c r="N78" s="81"/>
-      <c r="O78" s="82"/>
-    </row>
-    <row r="79" spans="1:15" ht="15" thickBot="1">
-      <c r="A79" s="40"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="51"/>
+      <c r="M78" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="N78" s="41"/>
+      <c r="O78" s="79"/>
+    </row>
+    <row r="79" spans="1:15" ht="15.6">
+      <c r="A79" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="57">
+        <v>1</v>
+      </c>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="50"/>
       <c r="L79"/>
-    </row>
-    <row r="80" spans="1:15" ht="15" thickTop="1">
-      <c r="A80" s="2"/>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="1:14">
-      <c r="E81" s="18"/>
-      <c r="K81" s="1"/>
-    </row>
-    <row r="82" spans="1:14">
-      <c r="E82" s="18"/>
-      <c r="K82" s="1"/>
-    </row>
-    <row r="83" spans="1:14">
-      <c r="E83" s="18"/>
-      <c r="K83" s="1"/>
-      <c r="N83"/>
-    </row>
-    <row r="84" spans="1:14">
-      <c r="E84" s="18"/>
-      <c r="K84" s="1"/>
-      <c r="N84"/>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="M79" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="N79" s="10"/>
+      <c r="O79" s="79"/>
+    </row>
+    <row r="80" spans="1:15" ht="15.6">
+      <c r="A80" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="57">
+        <v>3</v>
+      </c>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
+      <c r="K80" s="50"/>
+      <c r="L80"/>
+      <c r="M80" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="N80" s="10"/>
+      <c r="O80" s="79"/>
+    </row>
+    <row r="81" spans="1:15" ht="15.6">
+      <c r="A81" s="35"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="57"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="50"/>
+      <c r="L81"/>
+      <c r="M81" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="O81" s="79"/>
+    </row>
+    <row r="82" spans="1:15" ht="15" thickBot="1">
+      <c r="A82" s="35"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="57"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="50"/>
+      <c r="L82"/>
+      <c r="M82" s="80"/>
+      <c r="N82" s="81"/>
+      <c r="O82" s="82"/>
+    </row>
+    <row r="83" spans="1:15" ht="15" thickBot="1">
+      <c r="A83" s="40"/>
+      <c r="B83" s="31"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="51"/>
+      <c r="L83"/>
+    </row>
+    <row r="84" spans="1:15" ht="15" thickTop="1">
+      <c r="A84" s="2"/>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:15">
       <c r="E85" s="18"/>
       <c r="K85" s="1"/>
-      <c r="N85"/>
-    </row>
-    <row r="86" spans="1:14">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86" s="61"/>
-      <c r="D86"/>
-      <c r="E86" s="42"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-      <c r="J86"/>
-      <c r="K86"/>
-      <c r="L86"/>
-      <c r="M86"/>
-      <c r="N86"/>
-    </row>
-    <row r="87" spans="1:14">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87" s="61"/>
-      <c r="D87"/>
-      <c r="E87" s="42"/>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="L87"/>
-      <c r="M87"/>
+    </row>
+    <row r="86" spans="1:15">
+      <c r="E86" s="18"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="E87" s="18"/>
+      <c r="K87" s="1"/>
       <c r="N87"/>
     </row>
-    <row r="88" spans="1:14">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88" s="61"/>
-      <c r="D88"/>
-      <c r="E88" s="42"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-      <c r="M88"/>
+    <row r="88" spans="1:15">
+      <c r="E88" s="18"/>
+      <c r="K88" s="1"/>
       <c r="N88"/>
     </row>
-    <row r="89" spans="1:14">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89" s="61"/>
-      <c r="D89"/>
-      <c r="E89" s="42"/>
-      <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="L89"/>
-      <c r="M89"/>
+    <row r="89" spans="1:15">
+      <c r="E89" s="18"/>
+      <c r="K89" s="1"/>
       <c r="N89"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:15">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90" s="61"/>
@@ -5040,7 +5058,7 @@
       <c r="M90"/>
       <c r="N90"/>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:15">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91" s="61"/>
@@ -5056,7 +5074,7 @@
       <c r="M91"/>
       <c r="N91"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:15">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92" s="61"/>
@@ -5072,7 +5090,7 @@
       <c r="M92"/>
       <c r="N92"/>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:15">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93" s="61"/>
@@ -5088,7 +5106,7 @@
       <c r="M93"/>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:15">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94" s="61"/>
@@ -5104,7 +5122,7 @@
       <c r="M94"/>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:15">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95" s="61"/>
@@ -5120,7 +5138,7 @@
       <c r="M95"/>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:15">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96" s="61"/>
@@ -5152,20 +5170,84 @@
       <c r="M97"/>
       <c r="N97"/>
     </row>
+    <row r="98" spans="1:14">
+      <c r="A98"/>
+      <c r="B98"/>
+      <c r="C98" s="61"/>
+      <c r="D98"/>
+      <c r="E98" s="42"/>
+      <c r="F98"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98"/>
+      <c r="M98"/>
+      <c r="N98"/>
+    </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="1" t="s">
+      <c r="A99"/>
+      <c r="B99"/>
+      <c r="C99" s="61"/>
+      <c r="D99"/>
+      <c r="E99" s="42"/>
+      <c r="F99"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99"/>
+      <c r="M99"/>
+      <c r="N99"/>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="A100"/>
+      <c r="B100"/>
+      <c r="C100" s="61"/>
+      <c r="D100"/>
+      <c r="E100" s="42"/>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="L100"/>
+      <c r="M100"/>
+      <c r="N100"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101" s="61"/>
+      <c r="D101"/>
+      <c r="E101" s="42"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101"/>
+      <c r="M101"/>
+      <c r="N101"/>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
-      <c r="A100" s="2" t="s">
+    <row r="104" spans="1:14">
+      <c r="A104" s="2" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="L57:L58"/>
+    <mergeCell ref="M57:M58"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.45" right="0.45" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
@@ -5174,7 +5256,7 @@
     <oddFooter>&amp;R&amp;8&amp;F</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="47" max="16383" man="1"/>
+    <brk id="51" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>